<commit_message>
Remove place of birth from loan request parameters; add ippisNumber field to ippis upload data
</commit_message>
<xml_diff>
--- a/src/assets/documents/ippis-upload-sample.xlsx
+++ b/src/assets/documents/ippis-upload-sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unwachukwu1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unwachukwu1\Documents\coding\gigs\dominion-loan-repayment-portal\src\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63416267-7C76-4732-92AE-97AC7AA1A22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3D83F5-FF53-4018-8736-7441A423F6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>STAFF_ID</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>ACCOUNT_NUMBER</t>
+  </si>
+  <si>
+    <t>IPPIS_NO</t>
   </si>
 </sst>
 </file>
@@ -436,58 +439,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC07977B-1539-4CC5-B012-73A94EE6BE35}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes: 1. auto populate organization of customer from ippis validation; 2. Show preview of loan monthly repayment and total repayment on loan request 3. Add employer organization to ippis data capture 4. Add feature to download data as csv to various modules
</commit_message>
<xml_diff>
--- a/src/assets/documents/ippis-upload-sample.xlsx
+++ b/src/assets/documents/ippis-upload-sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unwachukwu1\Documents\coding\gigs\dominion-loan-repayment-portal\src\assets\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unwachukwu1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3D83F5-FF53-4018-8736-7441A423F6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A69D0AA-B4DA-4E87-9A7F-89C6F26E85E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>STAFF_ID</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>IPPIS_NO</t>
+  </si>
+  <si>
+    <t>EMPLOYER</t>
   </si>
 </sst>
 </file>
@@ -439,15 +442,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC07977B-1539-4CC5-B012-73A94EE6BE35}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -458,42 +461,45 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>